<commit_message>
GDPR modification to constructor
</commit_message>
<xml_diff>
--- a/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/DataFiles/MIRA_Websites_URLs.xlsx
+++ b/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/DataFiles/MIRA_Websites_URLs.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="19">
   <si>
     <t>URL</t>
   </si>
@@ -42,6 +42,33 @@
   </si>
   <si>
     <t>Datenschutzerklärung</t>
+  </si>
+  <si>
+    <t>http://aposervice.bayer.de</t>
+  </si>
+  <si>
+    <t>http://radiologie.bayer.de</t>
+  </si>
+  <si>
+    <t>http://wuppertal.bayer.de</t>
+  </si>
+  <si>
+    <t>http://www.ms-gateway.de</t>
+  </si>
+  <si>
+    <t>http://www.rennie.de</t>
+  </si>
+  <si>
+    <t>http://gesundebienen.bayer.de</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>http://www.ilja-rogoff.de</t>
+  </si>
+  <si>
+    <t>http://www.aktren.de</t>
   </si>
 </sst>
 </file>
@@ -82,11 +109,58 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+  <cellXfs count="50">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
@@ -94,51 +168,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.359375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="18.28515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="20.671875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="15.1015625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.1015625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="15.1015625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="15.1015625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="15.1015625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.25390625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.1015625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.1015625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.1015625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.1015625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.1015625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.1484375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -160,6 +235,212 @@
       </c>
       <c r="H2" t="b">
         <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDPR update to footer check
</commit_message>
<xml_diff>
--- a/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/DataFiles/MIRA_Websites_URLs.xlsx
+++ b/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/DataFiles/MIRA_Websites_URLs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="9360" windowWidth="15870" xWindow="0" yWindow="2430"/>
+    <workbookView windowHeight="3195" windowWidth="12480" xWindow="0" yWindow="2430"/>
   </bookViews>
   <sheets>
     <sheet name="German Privacy Info" r:id="rId1" sheetId="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>URL</t>
   </si>
@@ -44,43 +44,25 @@
     <t>Cookie Acceptance Phrase</t>
   </si>
   <si>
+    <t>https://laif900.de</t>
+  </si>
+  <si>
+    <t>Datenschutz</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Datenschutzerklärung</t>
+  </si>
+  <si>
     <t>http://laif900balance.de</t>
   </si>
   <si>
-    <t>Datenschutz</t>
-  </si>
-  <si>
     <t>Not found</t>
   </si>
   <si>
     <t>http://depression-behandeln-natuerlich.de</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>http://initiative-gesunder-magen.de</t>
-  </si>
-  <si>
-    <t>German privacy statement name not found</t>
-  </si>
-  <si>
-    <t>http://laif900.de</t>
-  </si>
-  <si>
-    <t>http://www.influex.de</t>
-  </si>
-  <si>
-    <t>http://legaplus.bayer.de</t>
-  </si>
-  <si>
-    <t>Datenschutzerklärung</t>
-  </si>
-  <si>
-    <t>http://onkologisch.slides.bayer.de</t>
-  </si>
-  <si>
-    <t>http://phytohustil.de</t>
   </si>
 </sst>
 </file>
@@ -123,11 +105,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -466,14 +446,14 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E2" sqref="E2:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="39.66015625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="39.78125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.56640625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="15.1015625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.1015625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="15.1015625" collapsed="true"/>
@@ -513,7 +493,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -537,12 +517,12 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -566,183 +546,15 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update to AppliTools Test
</commit_message>
<xml_diff>
--- a/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/DataFiles/MIRA_Websites_URLs.xlsx
+++ b/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/DataFiles/MIRA_Websites_URLs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="93">
   <si>
     <t>URL</t>
   </si>
@@ -336,9 +336,10 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -2471,8 +2472,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="9.3046875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="29.40625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.3046875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.40625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Update to claritin facebook test
</commit_message>
<xml_diff>
--- a/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/DataFiles/MIRA_Websites_URLs.xlsx
+++ b/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/DataFiles/MIRA_Websites_URLs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="93">
   <si>
     <t>URL</t>
   </si>
@@ -336,9 +336,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2472,8 +2474,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.3046875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.40625" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.3046875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.40625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>